<commit_message>
migration to mac done
</commit_message>
<xml_diff>
--- a/Budget.xlsx
+++ b/Budget.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -498,6 +498,125 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>0</v>
+      </c>
+      <c r="B4" t="n">
+        <v>43.06</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>44445</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>0</v>
+      </c>
+      <c r="B5" t="n">
+        <v>43.06</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>44445</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>0</v>
+      </c>
+      <c r="B6" t="n">
+        <v>43.06</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>44445</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B7" t="n">
+        <v>43.06</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>44445</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>0</v>
+      </c>
+      <c r="B8" t="n">
+        <v>43.06</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>44445</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>0</v>
+      </c>
+      <c r="B9" t="n">
+        <v>43.06</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>44445</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>0</v>
+      </c>
+      <c r="B10" t="n">
+        <v>43.06</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>44445</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>